<commit_message>
gap test 100% 통과하는 model 2_5 만듬
</commit_message>
<xml_diff>
--- a/controllers/CL_TEST_8_action 5/data/Curriculum Yes ob origin world_1/Curriculum Yes ob origin world_1_Test_No_world/Curriculum Yes ob origin world_1_Test_No_world_Test_Result.xlsx
+++ b/controllers/CL_TEST_8_action 5/data/Curriculum Yes ob origin world_1/Curriculum Yes ob origin world_1_Test_No_world/Curriculum Yes ob origin world_1_Test_No_world_Test_Result.xlsx
@@ -448,13 +448,13 @@
         <v>40</v>
       </c>
       <c r="B2" t="n">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4">
@@ -476,13 +476,13 @@
     </row>
     <row r="5">
       <c r="B5" t="n">
-        <v>0.9</v>
+        <v>0.3</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>0.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>